<commit_message>
Final update to code
He terminado el código, agregué las funciones de todos los botones, así cómo algunas modificaciones que me ayudaron a desarrollar más rápido mi programa.

El programa ya guarda datos nuevos en la base de datos y los lee sin problema.
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Preguntas y Respuestas"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
   <si>
     <t>Matrícula</t>
   </si>
@@ -38,13 +38,16 @@
     <t>Roberto</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>A01709578</t>
   </si>
   <si>
     <t>num2</t>
   </si>
   <si>
-    <t>Michel</t>
+    <t>Ale</t>
   </si>
   <si>
     <t>A01709579</t>
@@ -53,7 +56,7 @@
     <t>num3</t>
   </si>
   <si>
-    <t>Ernesto</t>
+    <t>Lili</t>
   </si>
   <si>
     <t>A01709580</t>
@@ -62,25 +65,61 @@
     <t>num4</t>
   </si>
   <si>
+    <t>Sara</t>
+  </si>
+  <si>
+    <t>A01709581</t>
+  </si>
+  <si>
+    <t>num5</t>
+  </si>
+  <si>
+    <t>Fer</t>
+  </si>
+  <si>
+    <t>A01709582</t>
+  </si>
+  <si>
+    <t>num6</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>A01702484</t>
+  </si>
+  <si>
+    <t>num7</t>
+  </si>
+  <si>
+    <t>Ashanti</t>
+  </si>
+  <si>
+    <t>A01701324</t>
+  </si>
+  <si>
+    <t>num8</t>
+  </si>
+  <si>
+    <t>Sebas</t>
+  </si>
+  <si>
+    <t>A01707256</t>
+  </si>
+  <si>
+    <t>num9</t>
+  </si>
+  <si>
     <t>Clarissa</t>
   </si>
   <si>
-    <t>A01709581</t>
-  </si>
-  <si>
-    <t>num5</t>
+    <t>A01700000</t>
+  </si>
+  <si>
+    <t>num10</t>
   </si>
   <si>
     <t>Paco</t>
-  </si>
-  <si>
-    <t>A01709582</t>
-  </si>
-  <si>
-    <t>num6</t>
-  </si>
-  <si>
-    <t>Ale</t>
   </si>
   <si>
     <t>Preguntas</t>
@@ -178,13 +217,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -220,22 +265,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -243,8 +288,11 @@
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -550,132 +598,132 @@
   </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="57.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="24.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="57.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="24.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="6" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="6" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+        <v>38</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="6" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+        <v>40</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="6" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+        <v>42</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="6" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+        <v>44</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="6" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+        <v>46</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="6" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
+        <v>48</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="6" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
+        <v>50</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="6" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+        <v>52</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="6" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
+        <v>54</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="6" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
+        <v>56</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="6" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
+        <v>58</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="6" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
+        <v>60</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="6" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18">
+        <v>62</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="6" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -688,9 +736,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -700,7 +748,7 @@
     <col min="4" max="4" style="5" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -714,7 +762,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -724,78 +772,134 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
-      <c r="A3" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3">
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="3">
-        <v>6</v>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+      <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
+      <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>